<commit_message>
Better tranport emissions graph.
</commit_message>
<xml_diff>
--- a/chapters/ch08-Transportation/datasets/CO2_emissions_transport.xlsx
+++ b/chapters/ch08-Transportation/datasets/CO2_emissions_transport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/MCBook2021/chapters/ch08-Transportation/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch08-Transportation/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32668FAF-8657-044B-8289-6C689EF0CF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19543944-36E6-6941-ACF5-172ECF60B3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13120" yWindow="2980" windowWidth="38000" windowHeight="24580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="131">
   <si>
     <t>Table A-104:  Total U.S. Greenhouse Gas Emissions from Transportation and Mobile Sources (MMT CO2 Eq.)</t>
   </si>
@@ -423,6 +423,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Ships and Boats</t>
   </si>
 </sst>
 </file>
@@ -858,7 +861,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -891,7 +894,7 @@
         <v>38</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Added source for transportation GHG emissions.
</commit_message>
<xml_diff>
--- a/chapters/ch08-Transportation/datasets/CO2_emissions_transport.xlsx
+++ b/chapters/ch08-Transportation/datasets/CO2_emissions_transport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch08-Transportation/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/MCBook2021/chapters/ch08-Transportation/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19543944-36E6-6941-ACF5-172ECF60B3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F181DE6-B000-1942-9BC5-18982D3F338E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26880" yWindow="8200" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
   <si>
     <t>Table A-104:  Total U.S. Greenhouse Gas Emissions from Transportation and Mobile Sources (MMT CO2 Eq.)</t>
   </si>
@@ -419,13 +419,22 @@
     <t>Medium- and Heavy-Duty Trucks</t>
   </si>
   <si>
+    <t>https://www.epa.gov/ghgemissions/inventory-us-greenhouse-gas-emissions-and-sinks-1990-2019</t>
+  </si>
+  <si>
+    <t>2021 Annex 3 Part A- pg 50</t>
+  </si>
+  <si>
+    <t>To find these data, you can follow the link above and go to "2021 Annex 3 Part A" page A-205 of the pdf. </t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Ships and Boats</t>
+  </si>
+  <si>
     <t>Pipelines</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Ships and Boats</t>
   </si>
 </sst>
 </file>
@@ -436,7 +445,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -477,6 +486,19 @@
       <sz val="10"/>
       <name val="Calibri "/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -495,8 +517,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -516,12 +539,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -861,48 +885,47 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="8.83203125" style="15"/>
+    <col min="2" max="6" width="8.83203125" style="15"/>
     <col min="7" max="11" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="18" customFormat="1" ht="14">
-      <c r="A1" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:20" s="17" customFormat="1" ht="14">
+      <c r="A1" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="K1" s="17" t="s">
+      <c r="J1" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>90</v>
       </c>
       <c r="L1" s="16"/>
@@ -1718,10 +1741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:U93"/>
+  <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1730,20 +1753,35 @@
     <col min="2" max="16" width="8"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:21" ht="14">
+    <row r="1" spans="1:16">
+      <c r="A1" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="14">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="4" spans="1:16" ht="21">
+      <c r="A4" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:16">
       <c r="P6" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
         <v>126</v>
       </c>
@@ -1793,7 +1831,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1842,12 +1880,8 @@
       <c r="P8" s="5">
         <v>0.23</v>
       </c>
-      <c r="U8" s="20">
-        <f>O9+O35+O43+O49+O57+O59</f>
-        <v>1880.5000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1896,12 +1930,8 @@
       <c r="P9" s="5">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T9" s="20">
-        <f>O10+O15+O20+O27+O33</f>
-        <v>1555.6000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -1950,12 +1980,8 @@
       <c r="P10" s="5">
         <v>0.19</v>
       </c>
-      <c r="S10" s="19">
-        <f>SUM(O11:O14)</f>
-        <v>762.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
@@ -2005,7 +2031,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:16">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
@@ -2055,7 +2081,7 @@
         <v>-0.41</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:16">
       <c r="A13" s="7" t="s">
         <v>6</v>
       </c>
@@ -2105,7 +2131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:16">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -2155,7 +2181,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -2205,7 +2231,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:16">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
@@ -4346,6 +4372,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{F385DA9C-8666-49E1-815A-CFA425BE0B52}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4354,8 +4383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BB16"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AF9" sqref="AF9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BC1" sqref="BC1:BV1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
Crippa data and graph.
</commit_message>
<xml_diff>
--- a/chapters/ch08-Transportation/datasets/CO2_emissions_transport.xlsx
+++ b/chapters/ch08-Transportation/datasets/CO2_emissions_transport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/MCBook2021/chapters/ch08-Transportation/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F181DE6-B000-1942-9BC5-18982D3F338E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F55BDAE-48D4-8A48-B371-6ABDF12ABBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26880" yWindow="8200" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26880" yWindow="8200" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="3" r:id="rId1"/>
@@ -884,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
@@ -1743,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>

</xml_diff>